<commit_message>
Small changes in UML plans
</commit_message>
<xml_diff>
--- a/Assets/UML.xlsx
+++ b/Assets/UML.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>DB</t>
   </si>
@@ -54,15 +54,9 @@
     <t>Players[]</t>
   </si>
   <si>
-    <t>User withID()</t>
-  </si>
-  <si>
     <t>$user</t>
   </si>
   <si>
-    <t>?/Profile/user_withID/5</t>
-  </si>
-  <si>
     <t>Kills</t>
   </si>
   <si>
@@ -97,6 +91,15 @@
   </si>
   <si>
     <t>TotalAmountOfUsers()</t>
+  </si>
+  <si>
+    <t>userWithID()</t>
+  </si>
+  <si>
+    <t>?/Profile/userWithID/5</t>
+  </si>
+  <si>
+    <t>receiveUser()</t>
   </si>
 </sst>
 </file>
@@ -239,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -249,6 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1333,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J22"/>
+  <dimension ref="A2:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,47 +1354,52 @@
     <col min="11" max="11" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
+      <c r="C5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="4"/>
+      <c r="C6" s="5"/>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="5"/>
-      <c r="E7" s="4" t="s">
-        <v>21</v>
+      <c r="E7" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="6" t="s">
-        <v>25</v>
+      <c r="E8" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
@@ -1407,10 +1416,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>9</v>
@@ -1421,7 +1430,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="4"/>
       <c r="G12" s="4" t="s">
@@ -1446,37 +1455,37 @@
         <v>7</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D19" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G19" s="4"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G20" s="5"/>
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="4:10" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>